<commit_message>
edit readme and todo
</commit_message>
<xml_diff>
--- a/options-init.xlsx
+++ b/options-init.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="17235" windowHeight="6210"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>String \| Array</t>
+  </si>
+  <si>
+    <t>[CodePen](https://codepen.io/maiCoding/pen/OajRdb)</t>
   </si>
 </sst>
 </file>
@@ -513,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +557,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -639,7 +642,7 @@
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s">
         <v>26</v>
@@ -656,7 +659,7 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="E8" t="s">
         <v>27</v>
@@ -673,7 +676,7 @@
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
update options table and readme
</commit_message>
<xml_diff>
--- a/options-init.xlsx
+++ b/options-init.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -175,6 +175,18 @@
   </si>
   <si>
     <t>[CodePen](https://codepen.io/maiCoding/pen/OajRdb)</t>
+  </si>
+  <si>
+    <t>[CodePen](https://codepen.io/maiCoding/pen/oQeQWe)</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>[CodePen](https://codepen.io/maiCoding/pen/gQxZpJ)</t>
+  </si>
+  <si>
+    <t>[CodePen](https://codepen.io/maiCoding/pen/OajrdX)</t>
   </si>
 </sst>
 </file>
@@ -517,7 +529,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,7 +537,7 @@
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="52" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -574,7 +586,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
         <v>46</v>
@@ -591,7 +603,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
         <v>47</v>
@@ -608,7 +620,7 @@
         <v>1.6</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
         <v>48</v>
@@ -625,7 +637,7 @@
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
         <v>49</v>
@@ -693,7 +705,7 @@
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="E10" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
add demo2 files. change reference to old animation durations
</commit_message>
<xml_diff>
--- a/options-init.xlsx
+++ b/options-init.xlsx
@@ -532,7 +532,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +603,7 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D4" t="s">
         <v>49</v>
@@ -612,7 +612,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -620,7 +620,7 @@
         <v>22</v>
       </c>
       <c r="C5">
-        <v>1.6</v>
+        <v>1.3</v>
       </c>
       <c r="D5" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
create v1.0.1 branch and update goals in TODO
</commit_message>
<xml_diff>
--- a/options-init.xlsx
+++ b/options-init.xlsx
@@ -129,15 +129,6 @@
     <t>If true then firing an animation while an animation is already playing will queue the second animation behind the first one and fire when the first one finishes. You can only have one queued animation per instance at a time. Queuing a new one will replace the current one.</t>
   </si>
   <si>
-    <t>Accepts an Object that will pass options whenever you animate to the start phase. For a list of valid phase options refer to the [Options (Phase)](https://github.com/RealTayy/slice-revealer#options-phase) section.</t>
-  </si>
-  <si>
-    <t>Accepts an Object that will pass options whenever you animate to the halfway phase. For a list of valid phase options refer to the [Options (Phase)](https://github.com/RealTayy/slice-revealer#options-phase) section.</t>
-  </si>
-  <si>
-    <t>Accepts an Object that will pass options whenever you animate to the end phase. For a list of valid phase options refer to the [Options (Phase)](https://github.com/RealTayy/slice-revealer#options-phase) section.</t>
-  </si>
-  <si>
     <t>The number of slices.</t>
   </si>
   <si>
@@ -186,10 +177,19 @@
     <t>[CodePen](https://codepen.io/maiCoding/pen/vQddEz)</t>
   </si>
   <si>
-    <t>By default the position of the element that contains the Slive Revealer instance has `position: abosolute`. If true then container element will have `position: sticky`. Used when target has scrollable content.</t>
-  </si>
-  <si>
     <t>Sets the `z-index` of the instance's container element.</t>
+  </si>
+  <si>
+    <t>Accepts an Object that will pass options whenever you animate to the start phase. For a list of valid phase options refer to the [Options (Phase)](https://github.com/RealTayy/slice-revealer#options---phase-optional) section.</t>
+  </si>
+  <si>
+    <t>Accepts an Object that will pass options whenever you animate to the halfway phase. For a list of valid phase options refer to the [Options (Phase)](https://github.com/RealTayy/slice-revealer#options---phase-optional) section.</t>
+  </si>
+  <si>
+    <t>Accepts an Object that will pass options whenever you animate to the end phase. For a list of valid phase options refer to the [Options (Phase)](https://github.com/RealTayy/slice-revealer#options---phase-optional) section.</t>
+  </si>
+  <si>
+    <t>By default the position of the element that contains the Slice Revealer instance has `position: abosolute`. If true then container element will have `position: sticky`. Used when target has scrollable content.</t>
   </si>
 </sst>
 </file>
@@ -532,7 +532,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +572,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -589,10 +589,10 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -606,10 +606,10 @@
         <v>0.8</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -623,10 +623,10 @@
         <v>1.3</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -634,21 +634,21 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -657,10 +657,10 @@
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -668,13 +668,13 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
         <v>23</v>
@@ -685,13 +685,13 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
@@ -702,13 +702,13 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E10" t="s">
         <v>25</v>
@@ -719,16 +719,16 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -745,7 +745,7 @@
         <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -762,7 +762,7 @@
         <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -779,7 +779,7 @@
         <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -793,7 +793,7 @@
         <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="E15" t="s">
         <v>36</v>
@@ -801,7 +801,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
         <v>33</v>
@@ -810,15 +810,15 @@
         <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
         <v>21</v>
@@ -827,10 +827,10 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update README and CodePens
</commit_message>
<xml_diff>
--- a/options-init.xlsx
+++ b/options-init.xlsx
@@ -99,9 +99,6 @@
     <t>Example</t>
   </si>
   <si>
-    <t>[CodePen]()</t>
-  </si>
-  <si>
     <t>queueAnimation</t>
   </si>
   <si>
@@ -190,6 +187,9 @@
   </si>
   <si>
     <t>By default the position of the element that contains the Slice Revealer instance has `position: abosolute`. If true then container element will have `position: sticky`. Used when target has scrollable content.</t>
+  </si>
+  <si>
+    <t>[CodePen](https://codepen.io/maiCoding/pen/MzLBoB)</t>
   </si>
 </sst>
 </file>
@@ -531,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +572,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -589,10 +589,10 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -606,10 +606,10 @@
         <v>0.8</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -623,10 +623,10 @@
         <v>1.3</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -634,21 +634,21 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -657,10 +657,10 @@
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -668,13 +668,13 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
         <v>23</v>
@@ -685,13 +685,13 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
@@ -702,13 +702,13 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E10" t="s">
         <v>25</v>
@@ -719,106 +719,106 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="E13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
         <v>31</v>
       </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
         <v>21</v>
@@ -827,10 +827,10 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>